<commit_message>
Update Fri 29 Mar 2024 16:47:22 EDT
</commit_message>
<xml_diff>
--- a/describe_dipep_IE.xlsx
+++ b/describe_dipep_IE.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-5.255753997843125</v>
+        <v>-5.243076914316876</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9585432037906777</v>
+        <v>0.9029963013744673</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-11.85297</v>
+        <v>-9.1299198</v>
       </c>
     </row>
     <row r="6">

</xml_diff>